<commit_message>
Added to Recode file
Coded about 8 lines
</commit_message>
<xml_diff>
--- a/Production-Casemarking/Analysis - Post Blindcoding/EmbodimentHallRecode_Taylor.xlsx
+++ b/Production-Casemarking/Analysis - Post Blindcoding/EmbodimentHallRecode_Taylor.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="0" windowWidth="19740" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-4080" yWindow="0" windowWidth="18700" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6807" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6810" uniqueCount="643">
   <si>
     <t>Agent.Embod</t>
   </si>
@@ -2445,10 +2445,10 @@
   <dimension ref="A1:L1969"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F610" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F802" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I630" sqref="I630"/>
+      <selection pane="bottomRight" activeCell="I818" sqref="I818"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -23830,6 +23830,15 @@
       <c r="H630" t="s">
         <v>69</v>
       </c>
+      <c r="I630" s="1">
+        <v>0</v>
+      </c>
+      <c r="J630">
+        <v>1</v>
+      </c>
+      <c r="K630">
+        <v>0</v>
+      </c>
     </row>
     <row r="631" spans="1:11">
       <c r="A631" s="2">
@@ -23856,6 +23865,15 @@
       <c r="H631" t="s">
         <v>13</v>
       </c>
+      <c r="I631" s="1">
+        <v>0</v>
+      </c>
+      <c r="J631">
+        <v>1</v>
+      </c>
+      <c r="K631">
+        <v>0</v>
+      </c>
     </row>
     <row r="632" spans="1:11">
       <c r="A632" s="2">
@@ -25339,7 +25357,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="689" spans="1:8">
+    <row r="689" spans="1:11">
       <c r="A689" s="2">
         <v>0</v>
       </c>
@@ -25365,7 +25383,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="690" spans="1:8">
+    <row r="690" spans="1:11">
       <c r="A690" s="2">
         <v>0</v>
       </c>
@@ -25390,8 +25408,17 @@
       <c r="H690" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="691" spans="1:8">
+      <c r="I690" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="J690" t="s">
+        <v>349</v>
+      </c>
+      <c r="K690" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="691" spans="1:11">
       <c r="A691" s="2">
         <v>1</v>
       </c>
@@ -25416,8 +25443,17 @@
       <c r="H691" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="692" spans="1:8">
+      <c r="I691" s="1">
+        <v>0</v>
+      </c>
+      <c r="J691">
+        <v>1</v>
+      </c>
+      <c r="K691">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="692" spans="1:11">
       <c r="A692" s="2">
         <v>0</v>
       </c>
@@ -25442,8 +25478,17 @@
       <c r="H692" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="693" spans="1:8">
+      <c r="I692" s="1">
+        <v>1</v>
+      </c>
+      <c r="J692">
+        <v>0</v>
+      </c>
+      <c r="K692">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="693" spans="1:11">
       <c r="A693" s="2">
         <v>0</v>
       </c>
@@ -25468,8 +25513,17 @@
       <c r="H693" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="694" spans="1:8">
+      <c r="I693" s="1">
+        <v>0</v>
+      </c>
+      <c r="J693">
+        <v>1</v>
+      </c>
+      <c r="K693">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="694" spans="1:11">
       <c r="A694" s="2">
         <v>0</v>
       </c>
@@ -25495,7 +25549,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="695" spans="1:8">
+    <row r="695" spans="1:11">
       <c r="A695" s="2">
         <v>1</v>
       </c>
@@ -25521,7 +25575,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="696" spans="1:8">
+    <row r="696" spans="1:11">
       <c r="A696" s="2">
         <v>1</v>
       </c>
@@ -25547,7 +25601,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="697" spans="1:8">
+    <row r="697" spans="1:11">
       <c r="A697" s="2">
         <v>0</v>
       </c>
@@ -25573,7 +25627,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="698" spans="1:8">
+    <row r="698" spans="1:11">
       <c r="A698" s="2">
         <v>1</v>
       </c>
@@ -25599,7 +25653,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="699" spans="1:8">
+    <row r="699" spans="1:11">
       <c r="A699" s="2">
         <v>1</v>
       </c>
@@ -25625,7 +25679,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="700" spans="1:8">
+    <row r="700" spans="1:11">
       <c r="A700" s="2">
         <v>1</v>
       </c>
@@ -25651,7 +25705,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="701" spans="1:8">
+    <row r="701" spans="1:11">
       <c r="A701" s="2">
         <v>1</v>
       </c>
@@ -25677,7 +25731,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="702" spans="1:8">
+    <row r="702" spans="1:11">
       <c r="A702" s="2">
         <v>0</v>
       </c>
@@ -25703,7 +25757,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="703" spans="1:8">
+    <row r="703" spans="1:11">
       <c r="A703" s="2">
         <v>0</v>
       </c>
@@ -25729,7 +25783,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="704" spans="1:8">
+    <row r="704" spans="1:11">
       <c r="A704" s="2">
         <v>0</v>
       </c>
@@ -26171,7 +26225,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="721" spans="1:8">
+    <row r="721" spans="1:11">
       <c r="A721" s="2">
         <v>1</v>
       </c>
@@ -26197,7 +26251,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="722" spans="1:8">
+    <row r="722" spans="1:11">
       <c r="A722" s="2">
         <v>0</v>
       </c>
@@ -26222,8 +26276,17 @@
       <c r="H722" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="723" spans="1:8">
+      <c r="I722" s="1">
+        <v>0</v>
+      </c>
+      <c r="J722">
+        <v>0</v>
+      </c>
+      <c r="K722">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="723" spans="1:11">
       <c r="A723" s="2">
         <v>1</v>
       </c>
@@ -26248,8 +26311,17 @@
       <c r="H723" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="724" spans="1:8">
+      <c r="I723" s="1">
+        <v>1</v>
+      </c>
+      <c r="J723">
+        <v>1</v>
+      </c>
+      <c r="K723">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="724" spans="1:11">
       <c r="A724" s="2">
         <v>1</v>
       </c>
@@ -26274,8 +26346,17 @@
       <c r="H724" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="725" spans="1:8">
+      <c r="I724" s="1">
+        <v>1</v>
+      </c>
+      <c r="J724">
+        <v>0</v>
+      </c>
+      <c r="K724">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="725" spans="1:11">
       <c r="A725" s="2">
         <v>1</v>
       </c>
@@ -26300,8 +26381,17 @@
       <c r="H725" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="726" spans="1:8">
+      <c r="I725" s="1">
+        <v>1</v>
+      </c>
+      <c r="J725">
+        <v>1</v>
+      </c>
+      <c r="K725">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="726" spans="1:11">
       <c r="A726" s="2">
         <v>1</v>
       </c>
@@ -26327,7 +26417,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="727" spans="1:8">
+    <row r="727" spans="1:11">
       <c r="A727" s="2">
         <v>0</v>
       </c>
@@ -26353,7 +26443,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="728" spans="1:8">
+    <row r="728" spans="1:11">
       <c r="A728" s="2">
         <v>1</v>
       </c>
@@ -26379,7 +26469,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="729" spans="1:8">
+    <row r="729" spans="1:11">
       <c r="A729" s="2">
         <v>1</v>
       </c>
@@ -26405,7 +26495,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="730" spans="1:8">
+    <row r="730" spans="1:11">
       <c r="A730" s="2">
         <v>1</v>
       </c>
@@ -26431,7 +26521,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="731" spans="1:8">
+    <row r="731" spans="1:11">
       <c r="A731" s="2">
         <v>0</v>
       </c>
@@ -26457,7 +26547,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="732" spans="1:8">
+    <row r="732" spans="1:11">
       <c r="A732" s="2">
         <v>1</v>
       </c>
@@ -26483,7 +26573,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="733" spans="1:8">
+    <row r="733" spans="1:11">
       <c r="A733" s="2">
         <v>1</v>
       </c>
@@ -26509,7 +26599,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="734" spans="1:8">
+    <row r="734" spans="1:11">
       <c r="A734" s="2">
         <v>1</v>
       </c>
@@ -26535,7 +26625,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="735" spans="1:8">
+    <row r="735" spans="1:11">
       <c r="A735" s="2">
         <v>1</v>
       </c>
@@ -26561,7 +26651,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="736" spans="1:8">
+    <row r="736" spans="1:11">
       <c r="A736" s="2">
         <v>1</v>
       </c>
@@ -27419,7 +27509,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="769" spans="1:8">
+    <row r="769" spans="1:11">
       <c r="A769" s="2">
         <v>1</v>
       </c>
@@ -27445,7 +27535,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="770" spans="1:8">
+    <row r="770" spans="1:11">
       <c r="A770" s="2">
         <v>1</v>
       </c>
@@ -27470,8 +27560,17 @@
       <c r="H770" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="771" spans="1:8">
+      <c r="I770" s="1">
+        <v>1</v>
+      </c>
+      <c r="J770">
+        <v>1</v>
+      </c>
+      <c r="K770">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="771" spans="1:11">
       <c r="A771" s="2">
         <v>1</v>
       </c>
@@ -27496,8 +27595,17 @@
       <c r="H771" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="772" spans="1:8">
+      <c r="I771" s="1">
+        <v>1</v>
+      </c>
+      <c r="J771">
+        <v>1</v>
+      </c>
+      <c r="K771">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="772" spans="1:11">
       <c r="A772" s="2">
         <v>1</v>
       </c>
@@ -27522,8 +27630,17 @@
       <c r="H772" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="773" spans="1:8">
+      <c r="I772" s="1">
+        <v>1</v>
+      </c>
+      <c r="J772">
+        <v>1</v>
+      </c>
+      <c r="K772">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="773" spans="1:11">
       <c r="A773" s="2">
         <v>1</v>
       </c>
@@ -27548,8 +27665,17 @@
       <c r="H773" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="774" spans="1:8">
+      <c r="I773" s="1">
+        <v>1</v>
+      </c>
+      <c r="J773">
+        <v>1</v>
+      </c>
+      <c r="K773">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="774" spans="1:11">
       <c r="A774" s="2">
         <v>1</v>
       </c>
@@ -27575,7 +27701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="775" spans="1:8">
+    <row r="775" spans="1:11">
       <c r="A775" s="2">
         <v>0</v>
       </c>
@@ -27601,7 +27727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="776" spans="1:8">
+    <row r="776" spans="1:11">
       <c r="A776" s="2">
         <v>1</v>
       </c>
@@ -27627,7 +27753,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="777" spans="1:8">
+    <row r="777" spans="1:11">
       <c r="A777" s="2">
         <v>1</v>
       </c>
@@ -27653,7 +27779,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="778" spans="1:8">
+    <row r="778" spans="1:11">
       <c r="A778" s="2">
         <v>1</v>
       </c>
@@ -27679,7 +27805,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="779" spans="1:8">
+    <row r="779" spans="1:11">
       <c r="A779" s="2">
         <v>0</v>
       </c>
@@ -27705,7 +27831,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="780" spans="1:8">
+    <row r="780" spans="1:11">
       <c r="A780" s="2">
         <v>1</v>
       </c>
@@ -27731,7 +27857,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="781" spans="1:8">
+    <row r="781" spans="1:11">
       <c r="A781" s="2">
         <v>1</v>
       </c>
@@ -27757,7 +27883,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="782" spans="1:8">
+    <row r="782" spans="1:11">
       <c r="A782" s="2">
         <v>1</v>
       </c>
@@ -27783,7 +27909,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="783" spans="1:8">
+    <row r="783" spans="1:11">
       <c r="A783" s="2">
         <v>1</v>
       </c>
@@ -27809,7 +27935,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="784" spans="1:8">
+    <row r="784" spans="1:11">
       <c r="A784" s="2">
         <v>1</v>
       </c>
@@ -28667,7 +28793,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="817" spans="1:8">
+    <row r="817" spans="1:11">
       <c r="A817" s="2">
         <v>1</v>
       </c>
@@ -28693,7 +28819,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="818" spans="1:8">
+    <row r="818" spans="1:11">
       <c r="A818" s="2">
         <v>0</v>
       </c>
@@ -28718,8 +28844,17 @@
       <c r="H818" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="819" spans="1:8">
+      <c r="I818" s="1">
+        <v>0</v>
+      </c>
+      <c r="J818">
+        <v>1</v>
+      </c>
+      <c r="K818">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="819" spans="1:11">
       <c r="A819" s="2">
         <v>1</v>
       </c>
@@ -28744,8 +28879,17 @@
       <c r="H819" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="820" spans="1:8">
+      <c r="I819" s="1">
+        <v>1</v>
+      </c>
+      <c r="J819">
+        <v>1</v>
+      </c>
+      <c r="K819">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="820" spans="1:11">
       <c r="A820" s="2">
         <v>1</v>
       </c>
@@ -28770,8 +28914,17 @@
       <c r="H820" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="821" spans="1:8">
+      <c r="I820" s="1">
+        <v>1</v>
+      </c>
+      <c r="J820">
+        <v>1</v>
+      </c>
+      <c r="K820">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="821" spans="1:11">
       <c r="A821" s="2">
         <v>0</v>
       </c>
@@ -28796,8 +28949,17 @@
       <c r="H821" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="822" spans="1:8">
+      <c r="I821" s="1">
+        <v>0</v>
+      </c>
+      <c r="J821">
+        <v>1</v>
+      </c>
+      <c r="K821">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="822" spans="1:11">
       <c r="A822" s="2">
         <v>0</v>
       </c>
@@ -28823,7 +28985,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="823" spans="1:8">
+    <row r="823" spans="1:11">
       <c r="A823" s="2">
         <v>0</v>
       </c>
@@ -28849,7 +29011,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="824" spans="1:8">
+    <row r="824" spans="1:11">
       <c r="A824" s="2">
         <v>1</v>
       </c>
@@ -28875,7 +29037,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="825" spans="1:8">
+    <row r="825" spans="1:11">
       <c r="A825" s="2">
         <v>0</v>
       </c>
@@ -28901,7 +29063,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="826" spans="1:8">
+    <row r="826" spans="1:11">
       <c r="A826" s="2">
         <v>1</v>
       </c>
@@ -28927,7 +29089,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="827" spans="1:8">
+    <row r="827" spans="1:11">
       <c r="A827" s="2">
         <v>1</v>
       </c>
@@ -28953,7 +29115,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="828" spans="1:8">
+    <row r="828" spans="1:11">
       <c r="A828" s="2">
         <v>1</v>
       </c>
@@ -28979,7 +29141,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="829" spans="1:8">
+    <row r="829" spans="1:11">
       <c r="A829" s="2">
         <v>1</v>
       </c>
@@ -29005,7 +29167,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="830" spans="1:8">
+    <row r="830" spans="1:11">
       <c r="A830" s="2">
         <v>0</v>
       </c>
@@ -29031,7 +29193,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="831" spans="1:8">
+    <row r="831" spans="1:11">
       <c r="A831" s="2">
         <v>0</v>
       </c>
@@ -29057,7 +29219,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="832" spans="1:8">
+    <row r="832" spans="1:11">
       <c r="A832" s="2">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Fixed some previous codes on Recode File
Fixed/Changed some previous codes entered by me on Recode File
</commit_message>
<xml_diff>
--- a/Production-Casemarking/Analysis - Post Blindcoding/EmbodimentHallRecode_Taylor.xlsx
+++ b/Production-Casemarking/Analysis - Post Blindcoding/EmbodimentHallRecode_Taylor.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="120" windowWidth="16160" windowHeight="14940" tabRatio="500"/>
+    <workbookView xWindow="-4220" yWindow="100" windowWidth="16160" windowHeight="14940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6813" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6807" uniqueCount="643">
   <si>
     <t>Agent.Embod</t>
   </si>
@@ -2445,10 +2445,10 @@
   <dimension ref="A1:L1969"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G832" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F844" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K850" sqref="K850"/>
+      <selection pane="bottomRight" activeCell="I847" sqref="I847"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -29608,8 +29608,8 @@
       <c r="I795" s="1">
         <v>1</v>
       </c>
-      <c r="J795" t="s">
-        <v>349</v>
+      <c r="J795">
+        <v>0</v>
       </c>
       <c r="K795">
         <v>0</v>
@@ -29678,8 +29678,8 @@
       <c r="I797" s="1">
         <v>1</v>
       </c>
-      <c r="J797" t="s">
-        <v>349</v>
+      <c r="J797">
+        <v>0</v>
       </c>
       <c r="K797">
         <v>1</v>
@@ -29713,8 +29713,8 @@
       <c r="I798" s="1">
         <v>1</v>
       </c>
-      <c r="J798" t="s">
-        <v>349</v>
+      <c r="J798">
+        <v>0</v>
       </c>
       <c r="K798">
         <v>0</v>
@@ -29783,8 +29783,8 @@
       <c r="I800" s="1">
         <v>1</v>
       </c>
-      <c r="J800" t="s">
-        <v>349</v>
+      <c r="J800">
+        <v>0</v>
       </c>
       <c r="K800">
         <v>0</v>
@@ -29819,7 +29819,7 @@
         <v>1</v>
       </c>
       <c r="J801">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K801">
         <v>1</v>
@@ -29854,7 +29854,7 @@
         <v>1</v>
       </c>
       <c r="J802">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K802">
         <v>1</v>
@@ -29923,8 +29923,8 @@
       <c r="I804" s="1">
         <v>1</v>
       </c>
-      <c r="J804" t="s">
-        <v>349</v>
+      <c r="J804">
+        <v>0</v>
       </c>
       <c r="K804">
         <v>1</v>
@@ -30063,8 +30063,8 @@
       <c r="I808" s="1">
         <v>1</v>
       </c>
-      <c r="J808" t="s">
-        <v>349</v>
+      <c r="J808">
+        <v>0</v>
       </c>
       <c r="K808">
         <v>0</v>
@@ -31138,7 +31138,7 @@
         <v>0</v>
       </c>
       <c r="J841">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K841">
         <v>0</v>

</xml_diff>